<commit_message>
Agregado de archivo en item de configuración
</commit_message>
<xml_diff>
--- a/Material de Estudio/Template Caso de Prueba.xlsx
+++ b/Material de Estudio/Template Caso de Prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\Facu\Facu\ISW\Clases Practicas\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://frcutneduar-my.sharepoint.com/personal/80384_sistemas_frc_utn_edu_ar/Documents/Documentos/Universidad/ISW-4K1-GRUPO4/Material de Estudio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29082647-0089-4490-9464-3120231FE21A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29082647-0089-4490-9464-3120231FE21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8085" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -1587,9 +1587,9 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4154,8 +4154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4410,20 +4410,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4553,19 +4553,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>